<commit_message>
fim do segundo treinamento
Modelo com 86 na roc para dados de 2023
</commit_message>
<xml_diff>
--- a/saida.xlsx
+++ b/saida.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,12 +564,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>13/02/2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=01/01/2023&amp;jornal=701&amp;pagina=144</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=13/02/2023&amp;jornal=600&amp;pagina=3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -579,12 +579,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Aprova a Estrutura Regimental e o Quadro Demonstrativo dos Cargos em Comissão e das Funções de Confiança do Ministério da Educação e remaneja cargos em comissão e funções de confiança.</t>
+          <t xml:space="preserve"> Institui o Programa Diogo de Sant'Ana Pró-Catadoras e Pró-Catadores para a Reciclagem Popular e o Comitê Interministerial para Inclusão Socioeconômica de Catadoras e Catadores de Materiais Reutilizáveis e Recicláveis.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.342, DE 1º DE JANEIRO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.414, DE 13 DE FEVEREIRO DE 2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -599,32 +599,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>13/02/2023</t>
+          <t>15/02/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=13/02/2023&amp;jornal=600&amp;pagina=3</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=15/02/2023&amp;jornal=600&amp;pagina=23</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Decreto numerado</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Programa Diogo de Sant'Ana Pró-Catadoras e Pró-Catadores para a Reciclagem Popular e o Comitê Interministerial para Inclusão Socioeconômica de Catadoras e Catadores de Materiais Reutilizáveis e Recicláveis.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.414, DE 13 DE FEVEREIRO DE 2023</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Atos do Poder Executivo</t>
+          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -634,32 +634,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15/02/2023</t>
+          <t>16/02/2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=15/02/2023&amp;jornal=600&amp;pagina=23</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=16/02/2023&amp;jornal=600&amp;pagina=1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Dispõe sobre a programação orçamentária e financeira, estabelece o cronograma de execução mensal de desembolso do Poder Executivo federal para o exercício de 2023 e dá outras providências.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> DECRETO Nº 11.415, DE 16 DE FEVEREIRO DE 2023</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -669,32 +669,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16/02/2023</t>
+          <t>08/03/2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=16/02/2023&amp;jornal=600&amp;pagina=1</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=08/03/2023&amp;jornal=515&amp;pagina=107</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Decreto numerado</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dispõe sobre a programação orçamentária e financeira, estabelece o cronograma de execução mensal de desembolso do Poder Executivo federal para o exercício de 2023 e dá outras providências.</t>
+          <t xml:space="preserve"> Institui o Programa Nacional de Equidade de Gênero, Raça e Valorização das Trabalhadoras no Sistema Único de Saúde - SUS.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.415, DE 16 DE FEVEREIRO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA GM/MS Nº 230, DE 7 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Atos do Poder Executivo</t>
+          <t>Ministério da Saúde/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=08/03/2023&amp;jornal=515&amp;pagina=107</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=08/03/2023&amp;jornal=515&amp;pagina=11</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -719,17 +719,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Programa Nacional de Equidade de Gênero, Raça e Valorização das Trabalhadoras no Sistema Único de Saúde - SUS.</t>
+          <t xml:space="preserve"> Institui o Comitê de Gênero, Raça e Diversidade, no âmbito do Ministério da Cultura e entidades supervisionadas.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA GM/MS Nº 230, DE 7 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA MINC Nº 7, DE 7 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Ministério da Saúde/Gabinete da Ministra</t>
+          <t>Ministério da Cultura/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -739,32 +739,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>08/03/2023</t>
+          <t>09/03/2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=08/03/2023&amp;jornal=515&amp;pagina=11</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=09/03/2023&amp;jornal=515&amp;pagina=4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Comitê de Gênero, Raça e Diversidade, no âmbito do Ministério da Cultura e entidades supervisionadas.</t>
+          <t xml:space="preserve"> Regulamenta a Lei nº 14.133, de 1º de abril de 2021, para dispor sobre a exigência, em contratações públicas, de percentual mínimo de mão de obra constituída por mulheres vítimas de violência doméstica e sobre a utilização do desenvolvimento, pelo licitante, de ações de equidade entre mulheres e homens no ambiente de trabalho como critério de desempate em licitações, no âmbito da administração pública federal direta, autárquica e fundacional.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA MINC Nº 7, DE 7 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.430, DE 8 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Ministério da Cultura/Gabinete da Ministra</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -809,32 +809,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21/03/2023</t>
+          <t>14/03/2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=21/03/2023&amp;jornal=515&amp;pagina=16</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=14/03/2023&amp;jornal=515&amp;pagina=83</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Resolução</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dispõe sobre a instituição do Comitê Gestor do bem cultural reconhecido como Patrimônio Mundial pela UNESCO - Sítio Arqueológico Cais do Valongo.</t>
+          <t xml:space="preserve">Dispõe sobre a reestruturação da Comissão Intersetorial de Políticas de Promoção da Equidade (CIPPE). </t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA IPHAN Nº 88, DE 20 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> RESOLUÇÃO Nº 700, DE 14 DE SETEMBRO DE 2022</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Ministério da Cultura/Instituto do Patrimônio Histórico e Artístico Nacional</t>
+          <t>Ministério da Saúde/Conselho Nacional de Saúde</t>
         </is>
       </c>
     </row>
@@ -844,32 +844,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>22/03/2023</t>
+          <t>21/03/2023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=1</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=21/03/2023&amp;jornal=515&amp;pagina=16</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Decreto numerado</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Institui Grupo de Trabalho Interministerial para a elaboração do Programa Nacional de Ações Afirmativas.</t>
+          <t xml:space="preserve"> Dispõe sobre a instituição do Comitê Gestor do bem cultural reconhecido como Patrimônio Mundial pela UNESCO - Sítio Arqueológico Cais do Valongo.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.442, DE 21 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA IPHAN Nº 88, DE 20 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Atos do Poder Executivo</t>
+          <t>Ministério da Cultura/Instituto do Patrimônio Histórico e Artístico Nacional</t>
         </is>
       </c>
     </row>
@@ -894,12 +894,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dispõe sobre o preenchimento por pessoas negras de percentual mínimo de cargos em comissão e funções de confiança no âmbito da administração pública federal.</t>
+          <t>Institui Grupo de Trabalho Interministerial para a elaboração do Programa Nacional de Ações Afirmativas.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.443, DE 21 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.442, DE 21 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=2</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=1</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -929,12 +929,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Institui Grupo de Trabalho Interministerial para elaboração da proposta do Plano Juventude Negra Viva.</t>
+          <t xml:space="preserve"> Dispõe sobre o preenchimento por pessoas negras de percentual mínimo de cargos em comissão e funções de confiança no âmbito da administração pública federal.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.444, DE 21 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.443, DE 21 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=3</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -964,12 +964,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Institui Grupo de Trabalho Interministerial, no âmbito do Ministério da Igualdade Racial, com a finalidade de apresentar proposta para o desenvolvimento de Programa de Enfrentamento do Racismo Religioso e Redução da Violência e Discriminação contra Povos e Comunidades Tradicionais de Matriz Africana e Povos de Terreiros no Brasil.</t>
+          <t>Institui Grupo de Trabalho Interministerial para elaboração da proposta do Plano Juventude Negra Viva.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.446, DE 21 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.444, DE 21 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=3</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -999,12 +999,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Programa Aquilomba Brasil e o seu Comitê Gestor.</t>
+          <t xml:space="preserve"> Institui o Grupo de Trabalho Interministerial do Cais do Valongo.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.447, DE 21 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.445, DE 21 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1019,32 +1019,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>23/03/2023</t>
+          <t>22/03/2023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/03/2023&amp;jornal=515&amp;pagina=193</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=3</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Resolução</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Institui Grupo de Trabalho Interministerial, no âmbito do Ministério da Igualdade Racial, com a finalidade de apresentar proposta para o desenvolvimento de Programa de Enfrentamento do Racismo Religioso e Redução da Violência e Discriminação contra Povos e Comunidades Tradicionais de Matriz Africana e Povos de Terreiros no Brasil.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> DECRETO Nº 11.446, DE 21 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Ministério da Saúde/Agência Nacional de Saúde Suplementar</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -1054,12 +1054,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23/03/2023</t>
+          <t>22/03/2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/03/2023&amp;jornal=515&amp;pagina=3</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=22/03/2023&amp;jornal=515&amp;pagina=3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1069,12 +1069,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Conselho Nacional de Desenvolvimento Rural Sustentável.</t>
+          <t xml:space="preserve"> Institui o Programa Aquilomba Brasil e o seu Comitê Gestor.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.451, DE 22 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.447, DE 21 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1089,12 +1089,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>24/03/2023</t>
+          <t>23/03/2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/03/2023&amp;jornal=515&amp;pagina=39</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/03/2023&amp;jornal=515&amp;pagina=193</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1104,17 +1104,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Estabelece procedimentos de heteroidentificação complementar à autodeclaração de candidatos negros (pretos e pardos) e indígenas nos processos seletivos e concursos públicos da UFRN.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RESOLUÇÃO CONJUNTA Nº 5, DE 14 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Ministério da Educação/Universidade Federal do Rio Grande do Norte/Conselho de Ensino, Pesquisa e Extensão</t>
+          <t>Ministério da Saúde/Agência Nacional de Saúde Suplementar</t>
         </is>
       </c>
     </row>
@@ -1124,32 +1124,32 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>31/03/2023</t>
+          <t>23/03/2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=31/03/2023&amp;jornal=515&amp;pagina=50</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/03/2023&amp;jornal=515&amp;pagina=243</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Resolução</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Comitê Permanente de Gênero, Raça e Diversidade no âmbito do Ministério da Integração e do Desenvolvimento Regional (MIDR) e entidades vinculadas.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA Nº 1.258, DE 30 DE MARÇO DE 2023</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Ministério da Integração e do Desenvolvimento Regional/Gabinete do Ministro</t>
+          <t>Ministério da Saúde/Agência Nacional de Saúde Suplementar</t>
         </is>
       </c>
     </row>
@@ -1159,32 +1159,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>18/04/2023</t>
+          <t>23/03/2023</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=18/04/2023&amp;jornal=515&amp;pagina=207</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/03/2023&amp;jornal=515&amp;pagina=3</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Resolução</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Estabelece normas para o exercício  profissional em relação ao caráter laico da prática psicológica.</t>
+          <t xml:space="preserve"> Institui o Conselho Nacional de Desenvolvimento Rural Sustentável.</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RESOLUÇÃO Nº 7, DE 6 DE ABRIL DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.451, DE 22 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Entidades de Fiscalização do Exercício das Profissões Liberais/Conselho Federal de Psicologia</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -1194,32 +1194,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>19/04/2023</t>
+          <t>24/03/2023</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=19/04/2023&amp;jornal=515&amp;pagina=69</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/03/2023&amp;jornal=515&amp;pagina=39</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Resolução</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Aprova as Instruções Específicas para o Exame de Admissão ao Estágio de Adaptação de Oficiais Engenheiros da Aeronáutica do ano de 2024 (IE/EA EAOEAR 2024).</t>
+          <t>Estabelece procedimentos de heteroidentificação complementar à autodeclaração de candidatos negros (pretos e pardos) e indígenas nos processos seletivos e concursos públicos da UFRN.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA DIRENS Nº 326/DCR, DE 7 DE FEVEREIRO DE 2023</t>
+          <t xml:space="preserve"> RESOLUÇÃO CONJUNTA Nº 5, DE 14 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Ministério da Defesa/Comando da Aeronáutica/Comando-Geral do Pessoal/Diretoria de Ensino</t>
+          <t>Ministério da Educação/Universidade Federal do Rio Grande do Norte/Conselho de Ensino, Pesquisa e Extensão</t>
         </is>
       </c>
     </row>
@@ -1229,12 +1229,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24/04/2023</t>
+          <t>31/03/2023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/04/2023&amp;jornal=515&amp;pagina=37</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=31/03/2023&amp;jornal=515&amp;pagina=50</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1244,17 +1244,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Institui Grupo de Trabalho, no âmbito do Ministério da Gestão e da Inovação em Serviços Públicos, com a finalidade de elaborar orientações, diretrizes, subsídios e contribuições para o desenvolvimento de ações que aperfeiçoem a implementação da Lei nº 12.990, de 9 de junho de 2014.</t>
+          <t xml:space="preserve"> Institui o Comitê Permanente de Gênero, Raça e Diversidade no âmbito do Ministério da Integração e do Desenvolvimento Regional (MIDR) e entidades vinculadas.</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA MGI Nº 1.370, DE 19  DE ABRIL DE 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 1.258, DE 30 DE MARÇO DE 2023</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Ministério da Gestão e da Inovação em Serviços Públicos/Gabinete da Ministra</t>
+          <t>Ministério da Integração e do Desenvolvimento Regional/Gabinete do Ministro</t>
         </is>
       </c>
     </row>
@@ -1264,32 +1264,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>24/04/2023</t>
+          <t>18/04/2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/04/2023&amp;jornal=515&amp;pagina=3</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=18/04/2023&amp;jornal=515&amp;pagina=207</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Lei</t>
+          <t>Resolução</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Altera os arts. 39 e 49 da Lei nº 12.288, de 20 de julho de 2010 (Estatuto da Igualdade Racial), para determinar procedimentos e critérios de coleta de informações relativas à distribuição dos segmentos étnicos e raciais no mercado de trabalho.</t>
+          <t xml:space="preserve"> Estabelece normas para o exercício  profissional em relação ao caráter laico da prática psicológica.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LEI Nº 14.553, DE 20 DE ABRIL DE 2023</t>
+          <t xml:space="preserve"> RESOLUÇÃO Nº 7, DE 6 DE ABRIL DE 2023</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Atos do Poder Legislativo</t>
+          <t>Entidades de Fiscalização do Exercício das Profissões Liberais/Conselho Federal de Psicologia</t>
         </is>
       </c>
     </row>
@@ -1299,32 +1299,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26/04/2023</t>
+          <t>19/04/2023</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=26/04/2023&amp;jornal=515&amp;pagina=3</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=19/04/2023&amp;jornal=515&amp;pagina=69</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Decreto numerado</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui Grupo de Trabalho Interministerial com a finalidade de buscar alternativas para a titulação territorial das Comunidades Remanescentes de Quilombos de Alcântara.</t>
+          <t xml:space="preserve"> Aprova as Instruções Específicas para o Exame de Admissão ao Estágio de Adaptação de Oficiais Engenheiros da Aeronáutica do ano de 2024 (IE/EA EAOEAR 2024).</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECRETO Nº 11.502, DE 25 DE ABRIL DE 2023</t>
+          <t xml:space="preserve"> PORTARIA DIRENS Nº 326/DCR, DE 7 DE FEVEREIRO DE 2023</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Atos do Poder Executivo</t>
+          <t>Ministério da Defesa/Comando da Aeronáutica/Comando-Geral do Pessoal/Diretoria de Ensino</t>
         </is>
       </c>
     </row>
@@ -1334,12 +1334,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>08/05/2023</t>
+          <t>24/04/2023</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=08/05/2023&amp;jornal=515&amp;pagina=18</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/04/2023&amp;jornal=515&amp;pagina=37</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1349,17 +1349,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Altera a Portaria nº 907, de 11 de maio de 2022, que define período para a realização da V Conferência Nacional de Promoção da Igualdade Racial - V CONAPIR, e dá outras providências.</t>
+          <t>Institui Grupo de Trabalho, no âmbito do Ministério da Gestão e da Inovação em Serviços Públicos, com a finalidade de elaborar orientações, diretrizes, subsídios e contribuições para o desenvolvimento de ações que aperfeiçoem a implementação da Lei nº 12.990, de 9 de junho de 2014.</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA Nº 124, DE 5 DE MAIO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA MGI Nº 1.370, DE 19  DE ABRIL DE 2023</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Ministério da Igualdade Racial/Gabinete da Ministra</t>
+          <t>Ministério da Gestão e da Inovação em Serviços Públicos/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -1369,32 +1369,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>17/05/2023</t>
+          <t>26/04/2023</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=17/05/2023&amp;jornal=515&amp;pagina=18</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=26/04/2023&amp;jornal=515&amp;pagina=3</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Institui Grupo de Trabalho Interministerial com a finalidade de buscar alternativas para a titulação territorial das Comunidades Remanescentes de Quilombos de Alcântara.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA SEFIC/MINC Nº 238, DE 16 DE MAIO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.502, DE 25 DE ABRIL DE 2023</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Ministério da Cultura/Secretaria de Economia Criativa e Fomento Cultural</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -1404,32 +1404,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18/05/2023</t>
+          <t>06/04/2023</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=18/05/2023&amp;jornal=515&amp;pagina=7</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=06/04/2023&amp;jornal=601&amp;pagina=2</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui Grupo de Trabalho - Raça, Equidade e Direitos Humanos com o objetivo de discutir, avaliar e propor políticas públicas que fomentem a inclusão social com foco na promoção da participação social e da igualdade de gênero, étnica e racial.</t>
+          <t xml:space="preserve"> Altera o Decreto nº 9.894, de 27 de junho de 2019, que dispõe sobre o Comitê Intersetorial de Acompanhamento e Monitoramento da Política Nacional para a População em Situação de Rua.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA MCOM Nº 9.453, DE 16 DE MAIO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.472, DE 6 DE ABRIL DE 2023</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Ministério das Comunicações/Gabinete do Ministro</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -1439,12 +1439,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>25/05/2023</t>
+          <t>08/05/2023</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=25/05/2023&amp;jornal=515&amp;pagina=307</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=08/05/2023&amp;jornal=515&amp;pagina=18</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1454,17 +1454,17 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui a Comissão Nacional de Educação do Campo - Conec.</t>
+          <t xml:space="preserve"> Altera a Portaria nº 907, de 11 de maio de 2022, que define período para a realização da V Conferência Nacional de Promoção da Igualdade Racial - V CONAPIR, e dá outras providências.</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA Nº 990, DE 23 DE MAIO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 124, DE 5 DE MAIO DE 2023</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Ministério da Educação/Gabinete do Ministro</t>
+          <t>Ministério da Igualdade Racial/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -1474,12 +1474,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>29/05/2023</t>
+          <t>17/05/2023</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=29/05/2023&amp;jornal=515&amp;pagina=111</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=17/05/2023&amp;jornal=515&amp;pagina=18</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1489,17 +1489,17 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Abre ao Orçamento Fiscal da União, em favor do Ministério da Igualdade Racial, crédito suplementar no valor de R$ 5.000.000,00, para reforço de dotação constante da Lei Orçamentária vigente.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Portaria GM/MPO Nº 146, DE 26 DE maio DE 2023</t>
+          <t xml:space="preserve"> PORTARIA SEFIC/MINC Nº 238, DE 16 DE MAIO DE 2023</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
+          <t>Ministério da Cultura/Secretaria de Economia Criativa e Fomento Cultural</t>
         </is>
       </c>
     </row>
@@ -1509,12 +1509,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>12/05/2023</t>
+          <t>18/05/2023</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=12/05/2023&amp;jornal=600&amp;pagina=57</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=18/05/2023&amp;jornal=515&amp;pagina=7</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1524,17 +1524,17 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Institui Grupo de Trabalho - Raça, Equidade e Direitos Humanos com o objetivo de discutir, avaliar e propor políticas públicas que fomentem a inclusão social com foco na promoção da participação social e da igualdade de gênero, étnica e racial.</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> PORTARIA MCOM Nº 9.453, DE 16 DE MAIO DE 2023</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
+          <t>Ministério das Comunicações/Gabinete do Ministro</t>
         </is>
       </c>
     </row>
@@ -1544,32 +1544,32 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>02/06/2023</t>
+          <t>25/05/2023</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=02/06/2023&amp;jornal=515&amp;pagina=276</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=25/05/2023&amp;jornal=515&amp;pagina=306</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Resolução</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Altera o Regimento Interno do Conselho de Arquitetura e Urbanismo do Brasil (CAU/BR), anexo à Resolução CAU/BR n° 139, de 28 de abril de 2017, e dá outras providências.</t>
+          <t xml:space="preserve"> Institui a Comissão Nacional de Educação Escolar Quilombola - Coneeq.</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RESOLUÇÃO Nº 234, DE 18 DE MAIO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 988, DE 23 DE MAIO DE 2023</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Entidades de Fiscalização do Exercício das Profissões Liberais/Conselho de Arquitetura e Urbanismo do Brasil</t>
+          <t>Ministério da Educação/Gabinete do Ministro</t>
         </is>
       </c>
     </row>
@@ -1579,12 +1579,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>05/06/2023</t>
+          <t>25/05/2023</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=05/06/2023&amp;jornal=515&amp;pagina=240</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=25/05/2023&amp;jornal=515&amp;pagina=307</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1594,17 +1594,17 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Institui a Comissão Nacional de Educação do Campo - Conec.</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA CPCIND/SENAJUS/MJSP Nº 787, DE 2 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 990, DE 23 DE MAIO DE 2023</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Ministério da Justiça e Segurança Pública/Secretaria Nacional de Justiça/Gabinete/Coordenação de Política de Classificação Indicativa</t>
+          <t>Ministério da Educação/Gabinete do Ministro</t>
         </is>
       </c>
     </row>
@@ -1614,32 +1614,32 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06/06/2023</t>
+          <t>29/05/2023</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=06/06/2023&amp;jornal=515&amp;pagina=5</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=29/05/2023&amp;jornal=515&amp;pagina=111</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Ação Direta de Inconstitucionalidade e Ação Declaratória de Constitucionalidade</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Abre ao Orçamento Fiscal da União, em favor do Ministério da Igualdade Racial, crédito suplementar no valor de R$ 5.000.000,00, para reforço de dotação constante da Lei Orçamentária vigente.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DECISÕES</t>
+          <t xml:space="preserve"> Portaria GM/MPO Nº 146, DE 26 DE maio DE 2023</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Atos do Poder Judiciário/Supremo Tribunal Federal/Plenário</t>
+          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -1649,12 +1649,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>07/06/2023</t>
+          <t>12/05/2023</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=07/06/2023&amp;jornal=515&amp;pagina=151</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=12/05/2023&amp;jornal=600&amp;pagina=57</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1664,17 +1664,17 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o Comitê Permanente de Governança da Participação Social, Diversidade e Inclusão no âmbito do Ministério da Pesca e Aquicultura.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Portaria MPA  nº 90, de 5 de junho de 2023</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Ministério da Pesca e Aquicultura/Gabinete do Ministro</t>
+          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -1684,32 +1684,32 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>13/06/2023</t>
+          <t>02/06/2023</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=13/06/2023&amp;jornal=515&amp;pagina=31</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=02/06/2023&amp;jornal=515&amp;pagina=276</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Resolução</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Delega competências à Secretária Executiva do Ministério da Igualdade Racial para realização de atos administrativos.</t>
+          <t>Altera o Regimento Interno do Conselho de Arquitetura e Urbanismo do Brasil (CAU/BR), anexo à Resolução CAU/BR n° 139, de 28 de abril de 2017, e dá outras providências.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA Nº 168, DE 12 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> RESOLUÇÃO Nº 234, DE 18 DE MAIO DE 2023</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Ministério da Igualdade Racial/Gabinete da Ministra</t>
+          <t>Entidades de Fiscalização do Exercício das Profissões Liberais/Conselho de Arquitetura e Urbanismo do Brasil</t>
         </is>
       </c>
     </row>
@@ -1719,32 +1719,32 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>15/06/2023</t>
+          <t>05/06/2023</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=15/06/2023&amp;jornal=515&amp;pagina=6</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=05/06/2023&amp;jornal=515&amp;pagina=240</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Lei</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui a Lei Geral do Esporte.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LEI Nº 14.597, DE 14 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA CPCIND/SENAJUS/MJSP Nº 787, DE 2 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Atos do Poder Legislativo</t>
+          <t>Ministério da Justiça e Segurança Pública/Secretaria Nacional de Justiça/Gabinete/Coordenação de Política de Classificação Indicativa</t>
         </is>
       </c>
     </row>
@@ -1754,32 +1754,32 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16/06/2023</t>
+          <t>06/06/2023</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=16/06/2023&amp;jornal=515&amp;pagina=14</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=06/06/2023&amp;jornal=515&amp;pagina=5</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Ação Direta de Inconstitucionalidade e Ação Declaratória de Constitucionalidade</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui o comitê permanente de gênero, raça e diversidade no âmbito do ministério de desenvolvimento e assistência social, família e combate à fome e dá outras providências.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA MDS Nº 892, DE 14 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> DECISÕES</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Ministério do Desenvolvimento e Assistência Social, Família e Combate à Fome/Gabinete do Ministro</t>
+          <t>Atos do Poder Judiciário/Supremo Tribunal Federal/Plenário</t>
         </is>
       </c>
     </row>
@@ -1789,12 +1789,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>19/06/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=19/06/2023&amp;jornal=515&amp;pagina=71</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=07/06/2023&amp;jornal=515&amp;pagina=151</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1804,17 +1804,17 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Institui Grupo de Trabalho Técnico com a finalidade de elaborar um plano de ação do governo federal para o combate ao racismo nas áreas de esporte e lazer. </t>
+          <t xml:space="preserve"> Institui o Comitê Permanente de Governança da Participação Social, Diversidade e Inclusão no âmbito do Ministério da Pesca e Aquicultura.</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve">    PORTARIA Nº 34, DE 16 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> Portaria MPA  nº 90, de 5 de junho de 2023</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Ministério do Esporte/Gabinete da Ministra</t>
+          <t>Ministério da Pesca e Aquicultura/Gabinete do Ministro</t>
         </is>
       </c>
     </row>
@@ -1824,12 +1824,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>23/06/2023</t>
+          <t>13/06/2023</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/06/2023&amp;jornal=515&amp;pagina=76</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=13/06/2023&amp;jornal=515&amp;pagina=31</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1839,12 +1839,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Torna pública a abertura de processo de consulta pública para a construção do Plano Juventude Negra Viva.</t>
+          <t>Delega competências à Secretária Executiva do Ministério da Igualdade Racial para realização de atos administrativos.</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA Nº 190, DE 22 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 168, DE 12 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1859,32 +1859,32 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>26/06/2023</t>
+          <t>15/06/2023</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=26/06/2023&amp;jornal=515&amp;pagina=160</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=15/06/2023&amp;jornal=515&amp;pagina=6</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Ata</t>
+          <t>Lei</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Institui a Lei Geral do Esporte.</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ATA Nº 19, DE 20 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> LEI Nº 14.597, DE 14 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Tribunal de Contas da União/2ª Câmara</t>
+          <t>Atos do Poder Legislativo</t>
         </is>
       </c>
     </row>
@@ -1894,12 +1894,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>29/06/2023</t>
+          <t>16/06/2023</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=29/06/2023&amp;jornal=515&amp;pagina=270</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=16/06/2023&amp;jornal=515&amp;pagina=14</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1909,17 +1909,17 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Define a estrutura de governança interna no âmbito do Ministério da Igualdade Racial e cria o Comitê de Governança Interna.</t>
+          <t xml:space="preserve"> Institui o comitê permanente de gênero, raça e diversidade no âmbito do ministério de desenvolvimento e assistência social, família e combate à fome e dá outras providências.</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA Nº 197, DE 28 DE JUNHO DE 2023</t>
+          <t xml:space="preserve"> PORTARIA MDS Nº 892, DE 14 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Ministério da Igualdade Racial/Gabinete da Ministra</t>
+          <t>Ministério do Desenvolvimento e Assistência Social, Família e Combate à Fome/Gabinete do Ministro</t>
         </is>
       </c>
     </row>
@@ -1929,12 +1929,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>05/07/2023</t>
+          <t>19/06/2023</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=05/07/2023&amp;jornal=515&amp;pagina=23</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=19/06/2023&amp;jornal=515&amp;pagina=71</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1944,17 +1944,17 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Convoca a 4ª Conferência Nacional de Cultura - 4ª CNC.</t>
+          <t xml:space="preserve">Institui Grupo de Trabalho Técnico com a finalidade de elaborar um plano de ação do governo federal para o combate ao racismo nas áreas de esporte e lazer. </t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA MINC Nº 41, DE 4 DE JULHO DE 2023</t>
+          <t xml:space="preserve">    PORTARIA Nº 34, DE 16 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Ministério da Cultura/Gabinete da Ministra</t>
+          <t>Ministério do Esporte/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -1964,32 +1964,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07/07/2023</t>
+          <t>23/06/2023</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=07/07/2023&amp;jornal=515&amp;pagina=137</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=23/06/2023&amp;jornal=515&amp;pagina=76</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Deliberação</t>
+          <t>Portaria</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Aprova o Regimento Interno do CAU/SP, e estabelece outras providências.</t>
+          <t>Torna pública a abertura de processo de consulta pública para a construção do Plano Juventude Negra Viva.</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DELIBERAÇÃO PLENÁRIA DPESP Nº 605-01, de 29 de junho de 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 190, DE 22 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Entidades de Fiscalização do Exercício das Profissões Liberais/Conselho de Arquitetura e Urbanismo de São Paulo</t>
+          <t>Ministério da Igualdade Racial/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -1999,12 +1999,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>26/06/2023</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=12/07/2023&amp;jornal=515&amp;pagina=41</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=26/06/2023&amp;jornal=515&amp;pagina=160</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2019,12 +2019,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t xml:space="preserve">  EXTRATO DA ATA DA 56ª REUNIÃO ORDINÁRIA REALIZADA EM 25 DE MAIO DE 2023</t>
+          <t xml:space="preserve"> ATA Nº 19, DE 20 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Ministério do Esporte/Gabinete da Ministra</t>
+          <t>Tribunal de Contas da União/2ª Câmara</t>
         </is>
       </c>
     </row>
@@ -2034,12 +2034,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>12/07/2023</t>
+          <t>29/06/2023</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=12/07/2023&amp;jornal=515&amp;pagina=71</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=29/06/2023&amp;jornal=515&amp;pagina=270</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2049,17 +2049,17 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Abre aos Orçamentos Fiscal e da Seguridade Social da União, em favor de diversos órgãos do Poder Executivo federal; e de Transferências a Estados, Distrito Federal e Municípios, crédito suplementar no valor de R$ 650.587.747,00, para reforço de dotações constantes da Lei Orçamentária vigente.</t>
+          <t>Define a estrutura de governança interna no âmbito do Ministério da Igualdade Racial e cria o Comitê de Governança Interna.</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Portaria GM/MPO Nº 188, DE 11 DE julho DE 2023</t>
+          <t xml:space="preserve"> PORTARIA Nº 197, DE 28 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
+          <t>Ministério da Igualdade Racial/Gabinete da Ministra</t>
         </is>
       </c>
     </row>
@@ -2069,32 +2069,32 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>24/07/2023</t>
+          <t>29/06/2023</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/07/2023&amp;jornal=515&amp;pagina=53</t>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=29/06/2023&amp;jornal=515&amp;pagina=2</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Portaria</t>
+          <t>Decreto numerado</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Institui a Política de Governança do Ministério do Desenvolvimento e Assistência Social, Família e Combate à Fome.</t>
+          <t xml:space="preserve"> Altera o Decreto nº 7.794, de 20 de agosto de 2012, que institui a Política Nacional de Agroecologia e Produção Orgânica, e o Decreto nº 6.323, de 27 de dezembro de 2007, para dispor sobre comissões com atuação na agricultura orgânica.</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PORTARIA MDS Nº 903, DE 21 DE JULHO DE 2023</t>
+          <t xml:space="preserve"> DECRETO Nº 11.582, DE 28 DE JUNHO DE 2023</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Ministério do Desenvolvimento e Assistência Social, Família e Combate à Fome/Gabinete do Ministro</t>
+          <t>Atos do Poder Executivo</t>
         </is>
       </c>
     </row>
@@ -2104,30 +2104,240 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>05/07/2023</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=05/07/2023&amp;jornal=515&amp;pagina=23</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Portaria</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Convoca a 4ª Conferência Nacional de Cultura - 4ª CNC.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PORTARIA MINC Nº 41, DE 4 DE JULHO DE 2023</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ministério da Cultura/Gabinete da Ministra</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=07/07/2023&amp;jornal=515&amp;pagina=137</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Deliberação</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Aprova o Regimento Interno do CAU/SP, e estabelece outras providências.</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> DELIBERAÇÃO PLENÁRIA DPESP Nº 605-01, de 29 de junho de 2023</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Entidades de Fiscalização do Exercício das Profissões Liberais/Conselho de Arquitetura e Urbanismo de São Paulo</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>12/07/2023</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=12/07/2023&amp;jornal=515&amp;pagina=41</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Ata</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  EXTRATO DA ATA DA 56ª REUNIÃO ORDINÁRIA REALIZADA EM 25 DE MAIO DE 2023</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Ministério do Esporte/Gabinete da Ministra</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>12/07/2023</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=12/07/2023&amp;jornal=515&amp;pagina=71</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Portaria</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Abre aos Orçamentos Fiscal e da Seguridade Social da União, em favor de diversos órgãos do Poder Executivo federal; e de Transferências a Estados, Distrito Federal e Municípios, crédito suplementar no valor de R$ 650.587.747,00, para reforço de dotações constantes da Lei Orçamentária vigente.</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Portaria GM/MPO Nº 188, DE 11 DE julho DE 2023</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Ministério do Planejamento e Orçamento/Gabinete da Ministra</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>18/07/2023</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=18/07/2023&amp;jornal=515&amp;pagina=12</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Ato</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>ATO Nº 32, DE 14 DE JULHO DE 2023</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Ministério da Agricultura e Pecuária/Secretaria de Defesa Agropecuária/Departamento de Sanidade Vegetal e Insumos Agrícolas/Coordenação-Geral de Agrotóxicos e Afins</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>24/07/2023</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=24/07/2023&amp;jornal=515&amp;pagina=53</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Portaria</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Institui a Política de Governança do Ministério do Desenvolvimento e Assistência Social, Família e Combate à Fome.</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> PORTARIA MDS Nº 903, DE 21 DE JULHO DE 2023</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Ministério do Desenvolvimento e Assistência Social, Família e Combate à Fome/Gabinete do Ministro</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>28/07/2023</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>http://pesquisa.in.gov.br/imprensa/jsp/visualiza/index.jsp?data=28/07/2023&amp;jornal=515&amp;pagina=48</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>Instrução Normativa</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t xml:space="preserve"> Disciplina a aplicação da reserva de vagas para pessoas negras nos concursos públicos, na forma da Lei n° 12.990, de 9 de junho de 2014, e reserva vagas para pessoas negras nos processos seletivos para a contratação por tempo determinado de que trata a Lei nº 8.745, de 9 de dezembro de 1993, no âmbito dos órgãos e entidades da administração pública federal direta, autárquica e fundacional.</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t xml:space="preserve"> INSTRUÇÃO NORMATIVA MGI Nº 23, DE 25 DE JULHO DE 2023</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G55" t="inlineStr">
         <is>
           <t>Ministério da Gestão e da Inovação em Serviços Públicos/Gabinete da Ministra</t>
         </is>

</xml_diff>